<commit_message>
bro thinks he's gaster
</commit_message>
<xml_diff>
--- a/usercode/experiments/documents.xlsx
+++ b/usercode/experiments/documents.xlsx
@@ -7,46 +7,46 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="norm" sheetId="1" r:id="rId1"/>
+    <sheet name="default" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="39">
   <si>
     <t>Chain Metrics</t>
   </si>
   <si>
-    <t>1923</t>
-  </si>
-  <si>
-    <t>4355</t>
-  </si>
-  <si>
-    <t>4166</t>
-  </si>
-  <si>
-    <t>3611</t>
-  </si>
-  <si>
-    <t>6389</t>
-  </si>
-  <si>
-    <t>0272</t>
-  </si>
-  <si>
-    <t>2635</t>
-  </si>
-  <si>
-    <t>2581</t>
-  </si>
-  <si>
-    <t>0372</t>
-  </si>
-  <si>
-    <t>6415</t>
+    <t>0000</t>
+  </si>
+  <si>
+    <t>0001</t>
+  </si>
+  <si>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>0003</t>
+  </si>
+  <si>
+    <t>0004</t>
+  </si>
+  <si>
+    <t>0005</t>
+  </si>
+  <si>
+    <t>0006</t>
+  </si>
+  <si>
+    <t>0007</t>
+  </si>
+  <si>
+    <t>0008</t>
+  </si>
+  <si>
+    <t>0009</t>
   </si>
   <si>
     <t>Average Within-Chain Similarity</t>
@@ -79,6 +79,9 @@
     <t>Global Minimum Within-Chain Similarity</t>
   </si>
   <si>
+    <t>Sum (testing)</t>
+  </si>
+  <si>
     <t>Clustering Metrics</t>
   </si>
   <si>
@@ -125,6 +128,9 @@
   </si>
   <si>
     <t>max_sentence_length</t>
+  </si>
+  <si>
+    <t>num_clusters</t>
   </si>
 </sst>
 </file>
@@ -490,7 +496,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -553,34 +559,34 @@
         <v>11</v>
       </c>
       <c r="B3" s="3">
-        <v>0.9370000000000001</v>
+        <v>0.945</v>
       </c>
       <c r="C3" s="3">
-        <v>0.951</v>
+        <v>0.9350000000000001</v>
       </c>
       <c r="D3" s="3">
-        <v>0.843</v>
+        <v>0.944</v>
       </c>
       <c r="E3" s="3">
-        <v>0.903</v>
+        <v>0.971</v>
       </c>
       <c r="F3" s="3">
-        <v>0.905</v>
+        <v>0.957</v>
       </c>
       <c r="G3" s="3">
-        <v>0.9419999999999999</v>
+        <v>0.957</v>
       </c>
       <c r="H3" s="3">
-        <v>0.921</v>
+        <v>0.965</v>
       </c>
       <c r="I3" s="3">
-        <v>0.917</v>
+        <v>0.982</v>
       </c>
       <c r="J3" s="3">
-        <v>0.95</v>
+        <v>0.965</v>
       </c>
       <c r="K3" s="3">
-        <v>0.9379999999999999</v>
+        <v>0.966</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -588,34 +594,34 @@
         <v>12</v>
       </c>
       <c r="B4" s="3">
-        <v>0.6700000166893005</v>
+        <v>0.6639999747276306</v>
       </c>
       <c r="C4" s="3">
-        <v>0.6499999761581421</v>
+        <v>0.675000011920929</v>
       </c>
       <c r="D4" s="3">
-        <v>0.6430000066757202</v>
+        <v>0.656000018119812</v>
       </c>
       <c r="E4" s="3">
-        <v>0.6179999709129333</v>
+        <v>0.6850000023841858</v>
       </c>
       <c r="F4" s="3">
-        <v>0.6439999938011169</v>
+        <v>0.6370000243186951</v>
       </c>
       <c r="G4" s="3">
-        <v>0.6179999709129333</v>
+        <v>0.6629999876022339</v>
       </c>
       <c r="H4" s="3">
-        <v>0.6959999799728394</v>
+        <v>0.6549999713897705</v>
       </c>
       <c r="I4" s="3">
-        <v>0.6850000023841858</v>
+        <v>0.6510000228881836</v>
       </c>
       <c r="J4" s="3">
-        <v>0.6859999895095825</v>
+        <v>0.6480000019073486</v>
       </c>
       <c r="K4" s="3">
-        <v>0.6389999985694885</v>
+        <v>0.6510000228881836</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -623,34 +629,34 @@
         <v>13</v>
       </c>
       <c r="B5" s="3">
-        <v>0.6340000033378601</v>
+        <v>0.6510000228881836</v>
       </c>
       <c r="C5" s="3">
-        <v>0.6290000081062317</v>
+        <v>0.6650000214576721</v>
       </c>
       <c r="D5" s="3">
-        <v>0.6259999871253967</v>
+        <v>0.6019999980926514</v>
       </c>
       <c r="E5" s="3">
-        <v>0.6029999852180481</v>
+        <v>0.7059999704360962</v>
       </c>
       <c r="F5" s="3">
+        <v>0.5970000028610229</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.6069999933242798</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.5770000219345093</v>
+      </c>
+      <c r="I5" s="3">
+        <v>0.5889999866485596</v>
+      </c>
+      <c r="J5" s="3">
         <v>0.6190000176429749</v>
       </c>
-      <c r="G5" s="3">
-        <v>0.5799999833106995</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0.675000011920929</v>
-      </c>
-      <c r="I5" s="3">
-        <v>0.6919999718666077</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0.6600000262260437</v>
-      </c>
       <c r="K5" s="3">
-        <v>0.6050000190734863</v>
+        <v>0.6320000290870667</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -658,34 +664,34 @@
         <v>14</v>
       </c>
       <c r="B6" s="3">
-        <v>0.6290000081062317</v>
+        <v>0.6079999804496765</v>
       </c>
       <c r="C6" s="3">
-        <v>0.6129999756813049</v>
+        <v>0.6759999990463257</v>
       </c>
       <c r="D6" s="3">
-        <v>0.6039999723434448</v>
+        <v>0.5910000205039978</v>
       </c>
       <c r="E6" s="3">
-        <v>0.5889999866485596</v>
+        <v>0.5740000009536743</v>
       </c>
       <c r="F6" s="3">
-        <v>0.5870000123977661</v>
+        <v>0.5789999961853027</v>
       </c>
       <c r="G6" s="3">
-        <v>0.5659999847412109</v>
+        <v>0.5090000033378601</v>
       </c>
       <c r="H6" s="3">
-        <v>0.6520000100135803</v>
+        <v>0.5329999923706055</v>
       </c>
       <c r="I6" s="3">
-        <v>0.6700000166893005</v>
+        <v>0.5910000205039978</v>
       </c>
       <c r="J6" s="3">
-        <v>0.6100000143051147</v>
+        <v>0.5929999947547913</v>
       </c>
       <c r="K6" s="3">
-        <v>0.5960000157356262</v>
+        <v>0.5680000185966492</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -693,34 +699,34 @@
         <v>15</v>
       </c>
       <c r="B7" s="3">
-        <v>0.6019999980926514</v>
+        <v>0.6060000061988831</v>
       </c>
       <c r="C7" s="3">
-        <v>0.5759999752044678</v>
+        <v>0.5770000219345093</v>
       </c>
       <c r="D7" s="3">
-        <v>0.5910000205039978</v>
+        <v>0.5600000023841858</v>
       </c>
       <c r="E7" s="3">
-        <v>0.5490000247955322</v>
+        <v>-1</v>
       </c>
       <c r="F7" s="3">
-        <v>0.5870000123977661</v>
+        <v>0.5680000185966492</v>
       </c>
       <c r="G7" s="3">
-        <v>0.5450000166893005</v>
+        <v>0.5090000033378601</v>
       </c>
       <c r="H7" s="3">
+        <v>0.5329999923706055</v>
+      </c>
+      <c r="I7" s="3">
         <v>-1</v>
       </c>
-      <c r="I7" s="3">
-        <v>0.6759999990463257</v>
-      </c>
       <c r="J7" s="3">
-        <v>0.5849999785423279</v>
+        <v>0.6940000057220459</v>
       </c>
       <c r="K7" s="3">
-        <v>0.6000000238418579</v>
+        <v>0.5680000185966492</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -728,34 +734,34 @@
         <v>16</v>
       </c>
       <c r="B8" s="3">
-        <v>0.6019999980926514</v>
+        <v>0.5759999752044678</v>
       </c>
       <c r="C8" s="3">
-        <v>0.5759999752044678</v>
+        <v>0.5540000200271606</v>
       </c>
       <c r="D8" s="3">
-        <v>0.5770000219345093</v>
+        <v>-1</v>
       </c>
       <c r="E8" s="3">
-        <v>0.5490000247955322</v>
+        <v>-1</v>
       </c>
       <c r="F8" s="3">
-        <v>0.5870000123977661</v>
+        <v>0.5419999957084656</v>
       </c>
       <c r="G8" s="3">
-        <v>0.5450000166893005</v>
+        <v>0.5090000033378601</v>
       </c>
       <c r="H8" s="3">
+        <v>0.5329999923706055</v>
+      </c>
+      <c r="I8" s="3">
         <v>-1</v>
       </c>
-      <c r="I8" s="3">
-        <v>0.6840000152587891</v>
-      </c>
       <c r="J8" s="3">
-        <v>0.5849999785423279</v>
+        <v>0.6940000057220459</v>
       </c>
       <c r="K8" s="3">
-        <v>0.6039999723434448</v>
+        <v>0.5379999876022339</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -763,34 +769,34 @@
         <v>17</v>
       </c>
       <c r="B9" s="3">
-        <v>0.6549999713897705</v>
+        <v>0.6100000143051147</v>
       </c>
       <c r="C9" s="3">
-        <v>0.6880000233650208</v>
+        <v>0.7250000238418579</v>
       </c>
       <c r="D9" s="3">
-        <v>0.6460000276565552</v>
+        <v>0.6010000109672546</v>
       </c>
       <c r="E9" s="3">
-        <v>0.6190000176429749</v>
+        <v>0.5740000009536743</v>
       </c>
       <c r="F9" s="3">
+        <v>0.6000000238418579</v>
+      </c>
+      <c r="G9" s="3">
         <v>-1</v>
       </c>
-      <c r="G9" s="3">
-        <v>0.6079999804496765</v>
-      </c>
       <c r="H9" s="3">
-        <v>0.6520000100135803</v>
+        <v>-1</v>
       </c>
       <c r="I9" s="3">
-        <v>0.6420000195503235</v>
+        <v>0.5910000205039978</v>
       </c>
       <c r="J9" s="3">
-        <v>0.621999979019165</v>
+        <v>0.492000013589859</v>
       </c>
       <c r="K9" s="3">
-        <v>0.5690000057220459</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -798,34 +804,34 @@
         <v>18</v>
       </c>
       <c r="B10" s="3">
-        <v>0.6520000100135803</v>
+        <v>0.6420000195503235</v>
       </c>
       <c r="C10" s="3">
-        <v>0.6259999871253967</v>
+        <v>0.6880000233650208</v>
       </c>
       <c r="D10" s="3">
-        <v>0.6389999985694885</v>
+        <v>0.6800000071525574</v>
       </c>
       <c r="E10" s="3">
-        <v>0.6269999742507935</v>
+        <v>0.6690000295639038</v>
       </c>
       <c r="F10" s="3">
-        <v>0.6340000033378601</v>
+        <v>0.6690000295639038</v>
       </c>
       <c r="G10" s="3">
-        <v>0.5860000252723694</v>
+        <v>0.6919999718666077</v>
       </c>
       <c r="H10" s="3">
-        <v>0.6299999952316284</v>
+        <v>0.609000027179718</v>
       </c>
       <c r="I10" s="3">
-        <v>0.6669999957084656</v>
+        <v>0.6899999976158142</v>
       </c>
       <c r="J10" s="3">
-        <v>0.6499999761581421</v>
+        <v>0.6949999928474426</v>
       </c>
       <c r="K10" s="3">
-        <v>0.6179999709129333</v>
+        <v>0.6529999971389771</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -833,34 +839,34 @@
         <v>19</v>
       </c>
       <c r="B11" s="3">
-        <v>1.369</v>
+        <v>1.302</v>
       </c>
       <c r="C11" s="3">
-        <v>1.513</v>
+        <v>1.411</v>
       </c>
       <c r="D11" s="3">
-        <v>3.146</v>
+        <v>1.324</v>
       </c>
       <c r="E11" s="3">
-        <v>1.824</v>
+        <v>1.125</v>
       </c>
       <c r="F11" s="3">
-        <v>1.488</v>
+        <v>1.319</v>
       </c>
       <c r="G11" s="3">
-        <v>1.347</v>
+        <v>1.209</v>
       </c>
       <c r="H11" s="3">
-        <v>1.444</v>
+        <v>1.327</v>
       </c>
       <c r="I11" s="3">
-        <v>1.737</v>
+        <v>1.071</v>
       </c>
       <c r="J11" s="3">
-        <v>1.277</v>
+        <v>1.17</v>
       </c>
       <c r="K11" s="3">
-        <v>1.485</v>
+        <v>1.199</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -868,117 +874,117 @@
         <v>20</v>
       </c>
       <c r="B12" s="3">
-        <v>0.401</v>
+        <v>0.227</v>
       </c>
       <c r="C12" s="3">
-        <v>0.188</v>
+        <v>0.238</v>
       </c>
       <c r="D12" s="3">
-        <v>0.08</v>
+        <v>0.213</v>
       </c>
       <c r="E12" s="3">
-        <v>0.304</v>
+        <v>0.472</v>
       </c>
       <c r="F12" s="3">
-        <v>0.318</v>
+        <v>0.189</v>
       </c>
       <c r="G12" s="3">
-        <v>0.399</v>
+        <v>0.214</v>
       </c>
       <c r="H12" s="3">
-        <v>0.399</v>
+        <v>0.309</v>
       </c>
       <c r="I12" s="3">
-        <v>0.417</v>
+        <v>0.48</v>
       </c>
       <c r="J12" s="3">
-        <v>0.401</v>
+        <v>0.225</v>
       </c>
       <c r="K12" s="3">
-        <v>0.278</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="1" t="s">
+        <v>0.221</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
+      <c r="B13" s="3">
+        <v>0.2809999883174896</v>
+      </c>
+      <c r="C13" s="3">
+        <v>4.184000015258789</v>
+      </c>
+      <c r="D13" s="3">
+        <v>7.560999870300293</v>
+      </c>
+      <c r="E13" s="3">
+        <v>12.58500003814697</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2.117000102996826</v>
+      </c>
+      <c r="G13" s="3">
+        <v>12.19099998474121</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1.845999956130981</v>
+      </c>
+      <c r="I13" s="3">
+        <v>7.221000194549561</v>
+      </c>
+      <c r="J13" s="3">
+        <v>2.865000009536743</v>
+      </c>
+      <c r="K13" s="3">
+        <v>14.74899959564209</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2" t="s">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="3">
-        <v>0.1780000030994415</v>
-      </c>
-      <c r="C16" s="3">
-        <v>0.1509999930858612</v>
-      </c>
-      <c r="D16" s="3">
-        <v>0.1620000004768372</v>
-      </c>
-      <c r="E16" s="3">
-        <v>0.2300000041723251</v>
-      </c>
-      <c r="F16" s="3">
-        <v>0.3100000023841858</v>
-      </c>
-      <c r="G16" s="3">
-        <v>0.164000004529953</v>
-      </c>
-      <c r="H16" s="3">
-        <v>0.2639999985694885</v>
-      </c>
-      <c r="I16" s="3">
-        <v>0.2829999923706055</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0.2460000067949295</v>
-      </c>
-      <c r="K16" s="3">
-        <v>0.2549999952316284</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -986,34 +992,34 @@
         <v>23</v>
       </c>
       <c r="B17" s="3">
-        <v>0.1790000051259995</v>
+        <v>0.1899999976158142</v>
       </c>
       <c r="C17" s="3">
-        <v>0.1140000000596046</v>
+        <v>0.1309999972581863</v>
       </c>
       <c r="D17" s="3">
-        <v>0.1209999993443489</v>
+        <v>0.2669999897480011</v>
       </c>
       <c r="E17" s="3">
-        <v>0.2179999947547913</v>
+        <v>0.1490000039339066</v>
       </c>
       <c r="F17" s="3">
-        <v>0.2709999978542328</v>
+        <v>0.1759999990463257</v>
       </c>
       <c r="G17" s="3">
-        <v>0.1729999929666519</v>
+        <v>0.1650000065565109</v>
       </c>
       <c r="H17" s="3">
-        <v>0.2770000100135803</v>
+        <v>0.1620000004768372</v>
       </c>
       <c r="I17" s="3">
-        <v>0.3729999959468842</v>
+        <v>0.1700000017881393</v>
       </c>
       <c r="J17" s="3">
-        <v>0.2419999986886978</v>
+        <v>0.2060000002384186</v>
       </c>
       <c r="K17" s="3">
-        <v>0.2290000021457672</v>
+        <v>0.1000000014901161</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1021,117 +1027,117 @@
         <v>24</v>
       </c>
       <c r="B18" s="3">
-        <v>0.024</v>
+        <v>0.1840000003576279</v>
       </c>
       <c r="C18" s="3">
-        <v>-0.01</v>
+        <v>0.1280000060796738</v>
       </c>
       <c r="D18" s="3">
+        <v>0.2709999978542328</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.1449999958276749</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.1410000026226044</v>
+      </c>
+      <c r="G18" s="3">
+        <v>0.1700000017881393</v>
+      </c>
+      <c r="H18" s="3">
+        <v>0.1449999958276749</v>
+      </c>
+      <c r="I18" s="3">
+        <v>0.1729999929666519</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0.2169999927282333</v>
+      </c>
+      <c r="K18" s="3">
+        <v>0.1089999973773956</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
+      <c r="A19" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="3">
+        <v>-0.004</v>
+      </c>
+      <c r="C19" s="3">
+        <v>-0.08599999999999999</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.017</v>
+      </c>
+      <c r="E19" s="3">
         <v>0</v>
       </c>
-      <c r="E18" s="3">
-        <v>0.005</v>
-      </c>
-      <c r="F18" s="3">
-        <v>0.03</v>
-      </c>
-      <c r="G18" s="3">
-        <v>-0.017</v>
-      </c>
-      <c r="H18" s="3">
-        <v>0.043</v>
-      </c>
-      <c r="I18" s="3">
-        <v>0.018</v>
-      </c>
-      <c r="J18" s="3">
-        <v>0.001</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0.013</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="F19" s="3">
+        <v>-0.018</v>
+      </c>
+      <c r="G19" s="3">
+        <v>-0.064</v>
+      </c>
+      <c r="H19" s="3">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>-0.224</v>
+      </c>
+      <c r="J19" s="3">
+        <v>-0.051</v>
+      </c>
+      <c r="K19" s="3">
+        <v>-0.014</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2" t="s">
+      <c r="A21" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" s="3">
-        <v>1923</v>
-      </c>
-      <c r="C22" s="3">
-        <v>4355</v>
-      </c>
-      <c r="D22" s="3">
-        <v>4166</v>
-      </c>
-      <c r="E22" s="3">
-        <v>3611</v>
-      </c>
-      <c r="F22" s="3">
-        <v>6389</v>
-      </c>
-      <c r="G22" s="3">
-        <v>272</v>
-      </c>
-      <c r="H22" s="3">
-        <v>2635</v>
-      </c>
-      <c r="I22" s="3">
-        <v>2581</v>
-      </c>
-      <c r="J22" s="3">
-        <v>372</v>
-      </c>
-      <c r="K22" s="3">
-        <v>6415</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1174,34 +1180,34 @@
         <v>28</v>
       </c>
       <c r="B24" s="3">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="C24" s="3">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="D24" s="3">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="E24" s="3">
-        <v>51</v>
+        <v>3</v>
       </c>
       <c r="F24" s="3">
-        <v>41</v>
+        <v>4</v>
       </c>
       <c r="G24" s="3">
-        <v>72</v>
+        <v>5</v>
       </c>
       <c r="H24" s="3">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="I24" s="3">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="J24" s="3">
-        <v>101</v>
+        <v>8</v>
       </c>
       <c r="K24" s="3">
-        <v>99</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1209,34 +1215,34 @@
         <v>29</v>
       </c>
       <c r="B25" s="3">
-        <v>1.369</v>
+        <v>159</v>
       </c>
       <c r="C25" s="3">
-        <v>1.513</v>
+        <v>151</v>
       </c>
       <c r="D25" s="3">
-        <v>3.146</v>
+        <v>68</v>
       </c>
       <c r="E25" s="3">
-        <v>1.824</v>
+        <v>88</v>
       </c>
       <c r="F25" s="3">
-        <v>1.488</v>
+        <v>119</v>
       </c>
       <c r="G25" s="3">
-        <v>1.347</v>
+        <v>110</v>
       </c>
       <c r="H25" s="3">
-        <v>1.444</v>
+        <v>49</v>
       </c>
       <c r="I25" s="3">
-        <v>1.737</v>
+        <v>156</v>
       </c>
       <c r="J25" s="3">
-        <v>1.277</v>
+        <v>112</v>
       </c>
       <c r="K25" s="3">
-        <v>1.485</v>
+        <v>196</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1244,34 +1250,34 @@
         <v>30</v>
       </c>
       <c r="B26" s="3">
-        <v>1</v>
+        <v>1.302</v>
       </c>
       <c r="C26" s="3">
-        <v>1</v>
+        <v>1.411</v>
       </c>
       <c r="D26" s="3">
-        <v>1</v>
+        <v>1.324</v>
       </c>
       <c r="E26" s="3">
-        <v>1</v>
+        <v>1.125</v>
       </c>
       <c r="F26" s="3">
-        <v>1</v>
+        <v>1.319</v>
       </c>
       <c r="G26" s="3">
-        <v>1</v>
+        <v>1.209</v>
       </c>
       <c r="H26" s="3">
-        <v>1</v>
+        <v>1.327</v>
       </c>
       <c r="I26" s="3">
-        <v>1</v>
+        <v>1.071</v>
       </c>
       <c r="J26" s="3">
-        <v>1</v>
+        <v>1.17</v>
       </c>
       <c r="K26" s="3">
-        <v>1</v>
+        <v>1.199</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1279,34 +1285,34 @@
         <v>31</v>
       </c>
       <c r="B27" s="3">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C27" s="3">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="D27" s="3">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="E27" s="3">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F27" s="3">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G27" s="3">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="H27" s="3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I27" s="3">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="J27" s="3">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="K27" s="3">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1314,34 +1320,34 @@
         <v>32</v>
       </c>
       <c r="B28" s="3">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="C28" s="3">
-        <v>174</v>
+        <v>9</v>
       </c>
       <c r="D28" s="3">
-        <v>129</v>
+        <v>5</v>
       </c>
       <c r="E28" s="3">
-        <v>93</v>
+        <v>4</v>
       </c>
       <c r="F28" s="3">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="G28" s="3">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="H28" s="3">
-        <v>78</v>
+        <v>12</v>
       </c>
       <c r="I28" s="3">
-        <v>99</v>
+        <v>4</v>
       </c>
       <c r="J28" s="3">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="K28" s="3">
-        <v>147</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1349,34 +1355,34 @@
         <v>33</v>
       </c>
       <c r="B29" s="3">
-        <v>4250</v>
+        <v>207</v>
       </c>
       <c r="C29" s="3">
-        <v>7562</v>
+        <v>213</v>
       </c>
       <c r="D29" s="3">
-        <v>5530</v>
+        <v>90</v>
       </c>
       <c r="E29" s="3">
-        <v>3417</v>
+        <v>99</v>
       </c>
       <c r="F29" s="3">
-        <v>2002</v>
+        <v>157</v>
       </c>
       <c r="G29" s="3">
-        <v>2827</v>
+        <v>133</v>
       </c>
       <c r="H29" s="3">
-        <v>2207</v>
+        <v>65</v>
       </c>
       <c r="I29" s="3">
-        <v>3832</v>
+        <v>167</v>
       </c>
       <c r="J29" s="3">
-        <v>3639</v>
+        <v>131</v>
       </c>
       <c r="K29" s="3">
-        <v>5716</v>
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1384,34 +1390,34 @@
         <v>34</v>
       </c>
       <c r="B30" s="3">
-        <v>36.957</v>
+        <v>5528</v>
       </c>
       <c r="C30" s="3">
-        <v>43.46</v>
+        <v>5893</v>
       </c>
       <c r="D30" s="3">
-        <v>42.868</v>
+        <v>2133</v>
       </c>
       <c r="E30" s="3">
-        <v>36.742</v>
+        <v>3561</v>
       </c>
       <c r="F30" s="3">
-        <v>32.82</v>
+        <v>3982</v>
       </c>
       <c r="G30" s="3">
-        <v>29.144</v>
+        <v>3848</v>
       </c>
       <c r="H30" s="3">
-        <v>28.295</v>
+        <v>3142</v>
       </c>
       <c r="I30" s="3">
-        <v>38.707</v>
+        <v>4903</v>
       </c>
       <c r="J30" s="3">
-        <v>28.209</v>
+        <v>3884</v>
       </c>
       <c r="K30" s="3">
-        <v>38.884</v>
+        <v>8024</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1419,34 +1425,34 @@
         <v>35</v>
       </c>
       <c r="B31" s="3">
-        <v>15</v>
+        <v>26.705</v>
       </c>
       <c r="C31" s="3">
-        <v>0</v>
+        <v>27.667</v>
       </c>
       <c r="D31" s="3">
-        <v>16</v>
+        <v>23.7</v>
       </c>
       <c r="E31" s="3">
-        <v>18</v>
+        <v>35.97</v>
       </c>
       <c r="F31" s="3">
-        <v>0</v>
+        <v>25.363</v>
       </c>
       <c r="G31" s="3">
-        <v>16</v>
+        <v>28.932</v>
       </c>
       <c r="H31" s="3">
-        <v>16</v>
+        <v>48.338</v>
       </c>
       <c r="I31" s="3">
-        <v>16</v>
+        <v>29.359</v>
       </c>
       <c r="J31" s="3">
-        <v>0</v>
+        <v>29.649</v>
       </c>
       <c r="K31" s="3">
-        <v>17</v>
+        <v>34.145</v>
       </c>
     </row>
     <row r="32" spans="1:11">
@@ -1454,41 +1460,111 @@
         <v>36</v>
       </c>
       <c r="B32" s="3">
-        <v>157</v>
+        <v>2</v>
       </c>
       <c r="C32" s="3">
-        <v>171</v>
+        <v>5</v>
       </c>
       <c r="D32" s="3">
+        <v>6</v>
+      </c>
+      <c r="E32" s="3">
+        <v>3</v>
+      </c>
+      <c r="F32" s="3">
+        <v>2</v>
+      </c>
+      <c r="G32" s="3">
+        <v>4</v>
+      </c>
+      <c r="H32" s="3">
+        <v>6</v>
+      </c>
+      <c r="I32" s="3">
+        <v>3</v>
+      </c>
+      <c r="J32" s="3">
+        <v>3</v>
+      </c>
+      <c r="K32" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="3">
+        <v>92</v>
+      </c>
+      <c r="C33" s="3">
+        <v>107</v>
+      </c>
+      <c r="D33" s="3">
+        <v>83</v>
+      </c>
+      <c r="E33" s="3">
+        <v>109</v>
+      </c>
+      <c r="F33" s="3">
+        <v>91</v>
+      </c>
+      <c r="G33" s="3">
+        <v>140</v>
+      </c>
+      <c r="H33" s="3">
         <v>167</v>
       </c>
-      <c r="E32" s="3">
-        <v>103</v>
-      </c>
-      <c r="F32" s="3">
-        <v>106</v>
-      </c>
-      <c r="G32" s="3">
-        <v>62</v>
-      </c>
-      <c r="H32" s="3">
-        <v>73</v>
-      </c>
-      <c r="I32" s="3">
-        <v>115</v>
-      </c>
-      <c r="J32" s="3">
-        <v>96</v>
-      </c>
-      <c r="K32" s="3">
-        <v>108</v>
+      <c r="I33" s="3">
+        <v>199</v>
+      </c>
+      <c r="J33" s="3">
+        <v>145</v>
+      </c>
+      <c r="K33" s="3">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="3">
+        <v>6</v>
+      </c>
+      <c r="C34" s="3">
+        <v>3</v>
+      </c>
+      <c r="D34" s="3">
+        <v>4</v>
+      </c>
+      <c r="E34" s="3">
+        <v>5</v>
+      </c>
+      <c r="F34" s="3">
+        <v>7</v>
+      </c>
+      <c r="G34" s="3">
+        <v>6</v>
+      </c>
+      <c r="H34" s="3">
+        <v>3</v>
+      </c>
+      <c r="I34" s="3">
+        <v>1</v>
+      </c>
+      <c r="J34" s="3">
+        <v>6</v>
+      </c>
+      <c r="K34" s="3">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A14:K14"/>
-    <mergeCell ref="A20:K20"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A21:K21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>